<commit_message>
Auto-committed on 2022/08/04 週四 11:38:29.36
</commit_message>
<xml_diff>
--- a/Program/Other/LM055_底稿_A042放款餘額彙總表.xlsx
+++ b/Program/Other/LM055_底稿_A042放款餘額彙總表.xlsx
@@ -5,11 +5,11 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\itxDoc\itxWrite\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A042填報說明" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <definedName name="_Order1" hidden="1">255</definedName>
     <definedName name="AS2DocOpenMode" hidden="1">"AS2DocumentEdit"</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">A042放款餘額彙總表!$B$1:$S$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">A042放款餘額彙總表!$B$1:$S$23</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">A042填報說明!$A$1:$G$24</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">A042填報說明!$1:$1</definedName>
     <definedName name="RiskAfterRecalcMacro" hidden="1">""</definedName>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="103">
   <si>
     <t>序號</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -2471,18 +2471,18 @@
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="4.90625" style="8" customWidth="1"/>
     <col min="2" max="2" width="25" style="8" customWidth="1"/>
-    <col min="3" max="3" width="7.77734375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" style="8" customWidth="1"/>
     <col min="5" max="6" width="22" style="8" customWidth="1"/>
-    <col min="7" max="7" width="36.77734375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="36.81640625" style="8" customWidth="1"/>
     <col min="8" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="32.4">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="34">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="32.4">
+    <row r="2" spans="1:7" ht="34">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2526,7 +2526,7 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="48.6">
+    <row r="3" spans="1:7" ht="51">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="48.6">
+    <row r="5" spans="1:7" ht="51">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="48.6">
+    <row r="8" spans="1:7" ht="51">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2726,7 +2726,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="32.4">
+    <row r="13" spans="1:7" ht="34">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2745,7 +2745,7 @@
       </c>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="32.4">
+    <row r="14" spans="1:7" ht="34">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2764,7 +2764,7 @@
       </c>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="32.4">
+    <row r="15" spans="1:7" ht="34">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="32.4">
+    <row r="16" spans="1:7" ht="34">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2802,7 +2802,7 @@
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" ht="32.4">
+    <row r="17" spans="1:7" ht="34">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2821,7 +2821,7 @@
       </c>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" ht="32.4">
+    <row r="18" spans="1:7" ht="34">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2840,7 +2840,7 @@
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" ht="32.4">
+    <row r="19" spans="1:7" ht="34">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2867,7 +2867,7 @@
       <c r="E20" s="15"/>
       <c r="F20" s="16"/>
     </row>
-    <row r="21" spans="1:7" ht="32.4">
+    <row r="21" spans="1:7" ht="34">
       <c r="A21" s="17" t="s">
         <v>50</v>
       </c>
@@ -2963,33 +2963,33 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="7" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" style="38" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="38" customWidth="1"/>
+    <col min="1" max="1" width="2.90625" style="38" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" style="38" customWidth="1"/>
     <col min="3" max="3" width="9" style="38" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="38" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="38" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" style="38" customWidth="1"/>
-    <col min="7" max="7" width="26.21875" style="38" customWidth="1"/>
-    <col min="8" max="8" width="24.88671875" style="38" customWidth="1"/>
-    <col min="9" max="9" width="17.77734375" style="38" customWidth="1"/>
-    <col min="10" max="10" width="21.44140625" style="38" customWidth="1"/>
-    <col min="11" max="12" width="12.6640625" style="38" customWidth="1"/>
-    <col min="13" max="13" width="17.88671875" style="38" customWidth="1"/>
-    <col min="14" max="15" width="17.33203125" style="38" customWidth="1"/>
-    <col min="16" max="17" width="15.6640625" style="38" customWidth="1"/>
-    <col min="18" max="18" width="24.21875" style="38" customWidth="1"/>
-    <col min="19" max="19" width="12.88671875" style="38" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" style="38" customWidth="1"/>
+    <col min="5" max="5" width="21.36328125" style="38" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" style="38" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" style="38" customWidth="1"/>
+    <col min="8" max="8" width="24.90625" style="38" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" style="38" customWidth="1"/>
+    <col min="10" max="10" width="21.453125" style="38" customWidth="1"/>
+    <col min="11" max="12" width="12.6328125" style="38" customWidth="1"/>
+    <col min="13" max="13" width="17.90625" style="38" customWidth="1"/>
+    <col min="14" max="15" width="17.36328125" style="38" customWidth="1"/>
+    <col min="16" max="17" width="15.6328125" style="38" customWidth="1"/>
+    <col min="18" max="18" width="24.1796875" style="38" customWidth="1"/>
+    <col min="19" max="19" width="12.90625" style="38" customWidth="1"/>
     <col min="20" max="16384" width="9" style="38"/>
   </cols>
   <sheetData>
@@ -3035,99 +3035,76 @@
     </row>
     <row r="5" spans="2:24">
       <c r="C5" s="39"/>
-      <c r="R5" s="71"/>
-      <c r="S5" s="71"/>
-    </row>
-    <row r="6" spans="2:24" s="42" customFormat="1" ht="48.6">
-      <c r="B6" s="41" t="s">
+      <c r="R5" s="36"/>
+      <c r="S5" s="37"/>
+    </row>
+    <row r="6" spans="2:24">
+      <c r="C6" s="39"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="71"/>
+    </row>
+    <row r="7" spans="2:24" s="42" customFormat="1" ht="51">
+      <c r="B7" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C7" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D7" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E7" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F7" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G7" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H7" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="41" t="s">
+      <c r="I7" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="J6" s="41" t="s">
+      <c r="J7" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="K6" s="41" t="s">
+      <c r="K7" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="L6" s="41" t="s">
+      <c r="L7" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="M6" s="41" t="s">
+      <c r="M7" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="N6" s="41" t="s">
+      <c r="N7" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="O6" s="41" t="s">
+      <c r="O7" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="P6" s="41" t="s">
+      <c r="P7" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="Q6" s="41" t="s">
+      <c r="Q7" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="R6" s="41" t="s">
+      <c r="R7" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="S6" s="41" t="s">
+      <c r="S7" s="41" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="2:24" s="46" customFormat="1" ht="15">
-      <c r="B7" s="43" t="s">
+    <row r="8" spans="2:24" s="46" customFormat="1" ht="15.5">
+      <c r="B8" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C8" s="43" t="s">
         <v>81</v>
-      </c>
-      <c r="D7" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
-      <c r="L7" s="63"/>
-      <c r="M7" s="63"/>
-      <c r="N7" s="63"/>
-      <c r="O7" s="63"/>
-      <c r="P7" s="63"/>
-      <c r="Q7" s="63"/>
-      <c r="R7" s="64"/>
-      <c r="S7" s="45"/>
-    </row>
-    <row r="8" spans="2:24" s="46" customFormat="1" ht="15">
-      <c r="B8" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>85</v>
       </c>
       <c r="D8" s="43" t="s">
         <v>82</v>
@@ -3150,9 +3127,9 @@
       <c r="R8" s="64"/>
       <c r="S8" s="45"/>
     </row>
-    <row r="9" spans="2:24" s="49" customFormat="1" ht="15">
+    <row r="9" spans="2:24" s="46" customFormat="1" ht="15.5">
       <c r="B9" s="43" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C9" s="43" t="s">
         <v>85</v>
@@ -3163,24 +3140,24 @@
       <c r="E9" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
       <c r="K9" s="63"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="47"/>
-      <c r="P9" s="47"/>
-      <c r="Q9" s="65"/>
-      <c r="R9" s="66"/>
-      <c r="S9" s="48"/>
-    </row>
-    <row r="10" spans="2:24" s="49" customFormat="1" ht="15">
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="64"/>
+      <c r="S9" s="45"/>
+    </row>
+    <row r="10" spans="2:24" s="49" customFormat="1" ht="15.5">
       <c r="B10" s="43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="43" t="s">
         <v>85</v>
@@ -3203,12 +3180,12 @@
       <c r="O10" s="47"/>
       <c r="P10" s="47"/>
       <c r="Q10" s="65"/>
-      <c r="R10" s="67"/>
-      <c r="S10" s="50"/>
-    </row>
-    <row r="11" spans="2:24" s="49" customFormat="1">
+      <c r="R10" s="66"/>
+      <c r="S10" s="48"/>
+    </row>
+    <row r="11" spans="2:24" s="49" customFormat="1" ht="15.5">
       <c r="B11" s="43" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C11" s="43" t="s">
         <v>85</v>
@@ -3216,8 +3193,8 @@
       <c r="D11" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="51" t="s">
-        <v>88</v>
+      <c r="E11" s="44" t="s">
+        <v>83</v>
       </c>
       <c r="F11" s="47"/>
       <c r="G11" s="47"/>
@@ -3232,253 +3209,309 @@
       <c r="P11" s="47"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="67"/>
-      <c r="S11" s="68" t="s">
+      <c r="S11" s="50"/>
+    </row>
+    <row r="12" spans="2:24" s="49" customFormat="1">
+      <c r="B12" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="67"/>
+      <c r="S12" s="68" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="2:24" s="49" customFormat="1" ht="15">
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="52"/>
-      <c r="S12" s="52"/>
-    </row>
-    <row r="13" spans="2:24" s="60" customFormat="1">
-      <c r="F13" s="62">
-        <f>SUM(F7:F12)</f>
+    <row r="13" spans="2:24" s="49" customFormat="1">
+      <c r="B13" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="65"/>
+      <c r="R13" s="67"/>
+      <c r="S13" s="68"/>
+    </row>
+    <row r="14" spans="2:24" s="49" customFormat="1" ht="15.5">
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="52"/>
+    </row>
+    <row r="15" spans="2:24" s="60" customFormat="1">
+      <c r="F15" s="62">
+        <f>SUM(F8:F14)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="62">
-        <f>SUM(G7:G12)</f>
+      <c r="G15" s="62">
+        <f>SUM(G8:G14)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="62">
-        <f>SUM(H7:H12)</f>
+      <c r="H15" s="62">
+        <f>SUM(H8:H14)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="62">
-        <f t="shared" ref="I13:Q13" si="0">SUM(I7:I12)</f>
+      <c r="I15" s="62">
+        <f>SUM(I8:I14)</f>
         <v>0</v>
       </c>
-      <c r="J13" s="62">
-        <f t="shared" si="0"/>
+      <c r="J15" s="62">
+        <f>SUM(J8:J14)</f>
         <v>0</v>
       </c>
-      <c r="K13" s="62">
-        <f t="shared" si="0"/>
+      <c r="K15" s="62">
+        <f>SUM(K8:K14)</f>
         <v>0</v>
       </c>
-      <c r="L13" s="62">
-        <f t="shared" si="0"/>
+      <c r="L15" s="62">
+        <f>SUM(L8:L14)</f>
         <v>0</v>
       </c>
-      <c r="M13" s="62">
-        <f>SUM(M7:M12)</f>
+      <c r="M15" s="62">
+        <f>SUM(M8:M14)</f>
         <v>0</v>
       </c>
-      <c r="N13" s="62">
-        <f t="shared" si="0"/>
+      <c r="N15" s="62">
+        <f>SUM(N8:N14)</f>
         <v>0</v>
       </c>
-      <c r="O13" s="62">
-        <f t="shared" si="0"/>
+      <c r="O15" s="62">
+        <f>SUM(O8:O14)</f>
         <v>0</v>
       </c>
-      <c r="P13" s="62">
-        <f t="shared" si="0"/>
+      <c r="P15" s="62">
+        <f>SUM(P8:P14)</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="62">
-        <f t="shared" si="0"/>
+      <c r="Q15" s="62">
+        <f>SUM(Q8:Q14)</f>
         <v>0</v>
       </c>
-      <c r="R13" s="61"/>
-    </row>
-    <row r="14" spans="2:24">
-      <c r="B14" s="53" t="s">
+      <c r="R15" s="61"/>
+    </row>
+    <row r="16" spans="2:24">
+      <c r="B16" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="56"/>
-      <c r="O14" s="56"/>
-      <c r="P14" s="56"/>
-      <c r="Q14" s="56"/>
-      <c r="R14" s="53"/>
-      <c r="S14" s="53"/>
-      <c r="T14" s="53"/>
-      <c r="U14" s="53"/>
-      <c r="V14" s="53"/>
-      <c r="W14" s="53"/>
-      <c r="X14" s="53"/>
-    </row>
-    <row r="15" spans="2:24">
-      <c r="B15" s="25" t="s">
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="53"/>
+      <c r="S16" s="53"/>
+      <c r="T16" s="53"/>
+      <c r="U16" s="53"/>
+      <c r="V16" s="53"/>
+      <c r="W16" s="53"/>
+      <c r="X16" s="53"/>
+    </row>
+    <row r="17" spans="1:25">
+      <c r="B17" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="53"/>
-      <c r="N15" s="53"/>
-      <c r="O15" s="53"/>
-      <c r="P15" s="53"/>
-      <c r="Q15" s="53"/>
-      <c r="R15" s="53"/>
-      <c r="S15" s="53"/>
-      <c r="T15" s="53"/>
-      <c r="U15" s="53"/>
-      <c r="V15" s="53"/>
-      <c r="W15" s="53"/>
-      <c r="X15" s="53"/>
-    </row>
-    <row r="16" spans="2:24" ht="35.25" customHeight="1">
-      <c r="B16" s="70" t="s">
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="53"/>
+      <c r="R17" s="53"/>
+      <c r="S17" s="53"/>
+      <c r="T17" s="53"/>
+      <c r="U17" s="53"/>
+      <c r="V17" s="53"/>
+      <c r="W17" s="53"/>
+      <c r="X17" s="53"/>
+    </row>
+    <row r="18" spans="1:25" ht="35.25" customHeight="1">
+      <c r="B18" s="70" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="70"/>
-      <c r="J16" s="70"/>
-      <c r="K16" s="70"/>
-      <c r="L16" s="70"/>
-      <c r="M16" s="70"/>
-      <c r="N16" s="70"/>
-      <c r="O16" s="70"/>
-      <c r="P16" s="70"/>
-      <c r="Q16" s="70"/>
-      <c r="R16" s="70"/>
-      <c r="S16" s="70"/>
-      <c r="T16" s="58"/>
-      <c r="U16" s="58"/>
-      <c r="V16" s="58"/>
-      <c r="W16" s="58"/>
-      <c r="X16" s="58"/>
-    </row>
-    <row r="17" spans="1:25" ht="16.5" customHeight="1">
-      <c r="B17" s="70" t="s">
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="70"/>
+      <c r="N18" s="70"/>
+      <c r="O18" s="70"/>
+      <c r="P18" s="70"/>
+      <c r="Q18" s="70"/>
+      <c r="R18" s="70"/>
+      <c r="S18" s="70"/>
+      <c r="T18" s="58"/>
+      <c r="U18" s="58"/>
+      <c r="V18" s="58"/>
+      <c r="W18" s="58"/>
+      <c r="X18" s="58"/>
+    </row>
+    <row r="19" spans="1:25" ht="16.5" customHeight="1">
+      <c r="B19" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="70"/>
-      <c r="L17" s="70"/>
-      <c r="M17" s="70"/>
-      <c r="N17" s="70"/>
-      <c r="O17" s="70"/>
-      <c r="P17" s="70"/>
-      <c r="Q17" s="70"/>
-      <c r="R17" s="70"/>
-      <c r="S17" s="58"/>
-      <c r="T17" s="58"/>
-      <c r="U17" s="58"/>
-      <c r="V17" s="58"/>
-      <c r="W17" s="58"/>
-      <c r="X17" s="58"/>
-    </row>
-    <row r="18" spans="1:25">
-      <c r="B18" s="53" t="s">
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="70"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="70"/>
+      <c r="P19" s="70"/>
+      <c r="Q19" s="70"/>
+      <c r="R19" s="70"/>
+      <c r="S19" s="58"/>
+      <c r="T19" s="58"/>
+      <c r="U19" s="58"/>
+      <c r="V19" s="58"/>
+      <c r="W19" s="58"/>
+      <c r="X19" s="58"/>
+    </row>
+    <row r="20" spans="1:25">
+      <c r="B20" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="53"/>
-      <c r="P18" s="53"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="53"/>
-      <c r="S18" s="53"/>
-      <c r="T18" s="53"/>
-      <c r="U18" s="53"/>
-      <c r="V18" s="53"/>
-      <c r="W18" s="53"/>
-      <c r="X18" s="53"/>
-    </row>
-    <row r="19" spans="1:25">
-      <c r="B19" s="38" t="s">
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="53"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="53"/>
+      <c r="R20" s="53"/>
+      <c r="S20" s="53"/>
+      <c r="T20" s="53"/>
+      <c r="U20" s="53"/>
+      <c r="V20" s="53"/>
+      <c r="W20" s="53"/>
+      <c r="X20" s="53"/>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="B21" s="38" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:25" s="26" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A21" s="59"/>
-      <c r="B21" s="26" t="s">
+    <row r="23" spans="1:25" s="26" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A23" s="59"/>
+      <c r="B23" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="28"/>
-      <c r="G21" s="31"/>
-      <c r="I21" s="31" t="s">
+      <c r="C23" s="27"/>
+      <c r="D23" s="28"/>
+      <c r="G23" s="31"/>
+      <c r="I23" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="J21" s="29"/>
-      <c r="K21" s="30"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="26" t="s">
+      <c r="J23" s="29"/>
+      <c r="K23" s="30"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="33"/>
-      <c r="T21" s="34"/>
-      <c r="W21" s="35"/>
-      <c r="Y21" s="26" t="s">
+      <c r="Q23" s="32"/>
+      <c r="R23" s="33"/>
+      <c r="T23" s="34"/>
+      <c r="W23" s="35"/>
+      <c r="Y23" s="26" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B16:S16"/>
-    <mergeCell ref="B17:R17"/>
-    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="B18:S18"/>
+    <mergeCell ref="B19:R19"/>
+    <mergeCell ref="R6:S6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Auto-committed on 2023/09/11 週一 11:46:57.72
</commit_message>
<xml_diff>
--- a/Program/Other/LM055_底稿_A042放款餘額彙總表.xlsx
+++ b/Program/Other/LM055_底稿_A042放款餘額彙總表.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\itxDoc\itxWrite\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKL_SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA8428B-558B-4136-8532-8D3CA8E1608C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7580" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A042填報說明" sheetId="1" r:id="rId1"/>
@@ -74,12 +75,12 @@
     <definedName name="TextRefCopyRangeCount" hidden="1">46</definedName>
     <definedName name="新">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="102">
   <si>
     <t>序號</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -729,10 +730,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Z</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>專案運用</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -740,7 +737,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -1654,99 +1651,87 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="35" fillId="0" borderId="2" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="35" fillId="0" borderId="2" xfId="39" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="2" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="180" fontId="12" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="12" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="12" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
@@ -1764,35 +1749,35 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="3" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="3" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="177" fontId="15" fillId="0" borderId="3" xfId="49" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1801,52 +1786,49 @@
     <xf numFmtId="178" fontId="15" fillId="0" borderId="2" xfId="49" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="15" fillId="0" borderId="2" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="8" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="46" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="15" fillId="0" borderId="3" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="3" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="3" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="177" fontId="15" fillId="0" borderId="2" xfId="49" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1861,119 +1843,119 @@
     <xf numFmtId="178" fontId="8" fillId="0" borderId="2" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="102">
-    <cellStyle name="20% - 輔色1 2 2" xfId="1"/>
-    <cellStyle name="20% - 輔色1 3 2" xfId="2"/>
-    <cellStyle name="20% - 輔色2 2 2" xfId="3"/>
-    <cellStyle name="20% - 輔色2 3 2" xfId="4"/>
-    <cellStyle name="20% - 輔色3 2 2" xfId="5"/>
-    <cellStyle name="20% - 輔色3 3 2" xfId="6"/>
-    <cellStyle name="20% - 輔色4 2 2" xfId="7"/>
-    <cellStyle name="20% - 輔色4 3 2" xfId="8"/>
-    <cellStyle name="20% - 輔色5 2 2" xfId="9"/>
-    <cellStyle name="20% - 輔色5 3 2" xfId="10"/>
-    <cellStyle name="20% - 輔色6 2 2" xfId="11"/>
-    <cellStyle name="20% - 輔色6 3 2" xfId="12"/>
-    <cellStyle name="40% - 輔色1 2 2" xfId="13"/>
-    <cellStyle name="40% - 輔色1 3 2" xfId="14"/>
-    <cellStyle name="40% - 輔色2 2 2" xfId="15"/>
-    <cellStyle name="40% - 輔色2 3 2" xfId="16"/>
-    <cellStyle name="40% - 輔色3 2 2" xfId="17"/>
-    <cellStyle name="40% - 輔色3 3 2" xfId="18"/>
-    <cellStyle name="40% - 輔色4 2 2" xfId="19"/>
-    <cellStyle name="40% - 輔色4 3 2" xfId="20"/>
-    <cellStyle name="40% - 輔色5 2 2" xfId="21"/>
-    <cellStyle name="40% - 輔色5 3 2" xfId="22"/>
-    <cellStyle name="40% - 輔色6 2 2" xfId="23"/>
-    <cellStyle name="40% - 輔色6 3 2" xfId="24"/>
-    <cellStyle name="60% - 輔色1 2 2" xfId="25"/>
-    <cellStyle name="60% - 輔色1 3 2" xfId="26"/>
-    <cellStyle name="60% - 輔色2 2 2" xfId="27"/>
-    <cellStyle name="60% - 輔色2 3 2" xfId="28"/>
-    <cellStyle name="60% - 輔色3 2 2" xfId="29"/>
-    <cellStyle name="60% - 輔色3 3 2" xfId="30"/>
-    <cellStyle name="60% - 輔色4 2 2" xfId="31"/>
-    <cellStyle name="60% - 輔色4 3 2" xfId="32"/>
-    <cellStyle name="60% - 輔色5 2 2" xfId="33"/>
-    <cellStyle name="60% - 輔色5 3 2" xfId="34"/>
-    <cellStyle name="60% - 輔色6 2 2" xfId="35"/>
-    <cellStyle name="60% - 輔色6 3 2" xfId="36"/>
+    <cellStyle name="20% - 輔色1 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - 輔色1 3 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - 輔色2 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - 輔色2 3 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - 輔色3 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - 輔色3 3 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="20% - 輔色4 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="20% - 輔色4 3 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - 輔色5 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="20% - 輔色5 3 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="20% - 輔色6 2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="20% - 輔色6 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="40% - 輔色1 2 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="40% - 輔色1 3 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="40% - 輔色2 2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="40% - 輔色2 3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="40% - 輔色3 2 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="40% - 輔色3 3 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="40% - 輔色4 2 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="40% - 輔色4 3 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="40% - 輔色5 2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="40% - 輔色5 3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="40% - 輔色6 2 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="40% - 輔色6 3 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="60% - 輔色1 2 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="60% - 輔色1 3 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="60% - 輔色2 2 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="60% - 輔色2 3 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="60% - 輔色3 2 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="60% - 輔色3 3 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="60% - 輔色4 2 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="60% - 輔色4 3 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="60% - 輔色5 2 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="60% - 輔色5 3 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="60% - 輔色6 2 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="60% - 輔色6 3 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 10" xfId="37"/>
-    <cellStyle name="一般 10 2" xfId="38"/>
-    <cellStyle name="一般 2" xfId="39"/>
-    <cellStyle name="一般 2 2" xfId="40"/>
-    <cellStyle name="一般 3" xfId="41"/>
-    <cellStyle name="一般 3 2" xfId="42"/>
-    <cellStyle name="一般 4" xfId="43"/>
-    <cellStyle name="一般 5" xfId="44"/>
-    <cellStyle name="一般 6" xfId="45"/>
-    <cellStyle name="一般_921002保險業月報yaotung" xfId="46"/>
-    <cellStyle name="一般_9211預月" xfId="47"/>
-    <cellStyle name="一般_半年報檢查報表-壽險" xfId="48"/>
+    <cellStyle name="一般 10" xfId="37" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="一般 10 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="一般 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="一般 2 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="一般 3" xfId="41" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="一般 3 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="一般 4" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="一般 5" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="一般 6" xfId="45" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="一般_921002保險業月報yaotung" xfId="46" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="一般_9211預月" xfId="47" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="一般_半年報檢查報表-壽險" xfId="48" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
     <cellStyle name="千分位" xfId="49" builtinId="3"/>
-    <cellStyle name="千分位 2" xfId="50"/>
-    <cellStyle name="千分位 3" xfId="51"/>
-    <cellStyle name="千分位 3 2" xfId="52"/>
-    <cellStyle name="千分位 4" xfId="53"/>
-    <cellStyle name="千分位[0] 2" xfId="54"/>
-    <cellStyle name="中等 2 2" xfId="55"/>
-    <cellStyle name="中等 3 2" xfId="56"/>
-    <cellStyle name="合計 2 2" xfId="57"/>
-    <cellStyle name="合計 3 2" xfId="58"/>
-    <cellStyle name="好 2 2" xfId="59"/>
-    <cellStyle name="好 3 2" xfId="60"/>
-    <cellStyle name="百分比 2" xfId="61"/>
-    <cellStyle name="計算方式 2 2" xfId="62"/>
-    <cellStyle name="計算方式 3 2" xfId="63"/>
-    <cellStyle name="連結的儲存格 2 2" xfId="64"/>
-    <cellStyle name="連結的儲存格 3 2" xfId="65"/>
-    <cellStyle name="備註 2 2" xfId="66"/>
-    <cellStyle name="備註 3 2" xfId="67"/>
-    <cellStyle name="說明文字 2 2" xfId="68"/>
-    <cellStyle name="說明文字 3 2" xfId="69"/>
-    <cellStyle name="輔色1 2 2" xfId="70"/>
-    <cellStyle name="輔色1 3 2" xfId="71"/>
-    <cellStyle name="輔色2 2 2" xfId="72"/>
-    <cellStyle name="輔色2 3 2" xfId="73"/>
-    <cellStyle name="輔色3 2 2" xfId="74"/>
-    <cellStyle name="輔色3 3 2" xfId="75"/>
-    <cellStyle name="輔色4 2 2" xfId="76"/>
-    <cellStyle name="輔色4 3 2" xfId="77"/>
-    <cellStyle name="輔色5 2 2" xfId="78"/>
-    <cellStyle name="輔色5 3 2" xfId="79"/>
-    <cellStyle name="輔色6 2 2" xfId="80"/>
-    <cellStyle name="輔色6 3 2" xfId="81"/>
-    <cellStyle name="標題 1 2 2" xfId="82"/>
-    <cellStyle name="標題 1 3 2" xfId="83"/>
-    <cellStyle name="標題 2 2 2" xfId="84"/>
-    <cellStyle name="標題 2 3 2" xfId="85"/>
-    <cellStyle name="標題 3 2 2" xfId="86"/>
-    <cellStyle name="標題 3 3 2" xfId="87"/>
-    <cellStyle name="標題 4 2 2" xfId="88"/>
-    <cellStyle name="標題 4 3 2" xfId="89"/>
-    <cellStyle name="標題 5 2" xfId="90"/>
-    <cellStyle name="標題 6 2" xfId="91"/>
-    <cellStyle name="輸入 2 2" xfId="92"/>
-    <cellStyle name="輸入 3 2" xfId="93"/>
-    <cellStyle name="輸出 2 2" xfId="94"/>
-    <cellStyle name="輸出 3 2" xfId="95"/>
-    <cellStyle name="檢查儲存格 2 2" xfId="96"/>
-    <cellStyle name="檢查儲存格 3 2" xfId="97"/>
-    <cellStyle name="壞 2 2" xfId="98"/>
-    <cellStyle name="壞 3 2" xfId="99"/>
-    <cellStyle name="警告文字 2 2" xfId="100"/>
-    <cellStyle name="警告文字 3 2" xfId="101"/>
+    <cellStyle name="千分位 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="千分位 3" xfId="51" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="千分位 3 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="千分位 4" xfId="53" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="千分位[0] 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="中等 2 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="中等 3 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="合計 2 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="合計 3 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="好 2 2" xfId="59" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="好 3 2" xfId="60" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="百分比 2" xfId="61" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="計算方式 2 2" xfId="62" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="計算方式 3 2" xfId="63" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="連結的儲存格 2 2" xfId="64" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="連結的儲存格 3 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="備註 2 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="備註 3 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="說明文字 2 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="說明文字 3 2" xfId="69" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="輔色1 2 2" xfId="70" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="輔色1 3 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="輔色2 2 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="輔色2 3 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="輔色3 2 2" xfId="74" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="輔色3 3 2" xfId="75" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="輔色4 2 2" xfId="76" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="輔色4 3 2" xfId="77" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="輔色5 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="輔色5 3 2" xfId="79" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="輔色6 2 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="輔色6 3 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="標題 1 2 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="標題 1 3 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="標題 2 2 2" xfId="84" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="標題 2 3 2" xfId="85" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="標題 3 2 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="標題 3 3 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="標題 4 2 2" xfId="88" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="標題 4 3 2" xfId="89" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="標題 5 2" xfId="90" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="標題 6 2" xfId="91" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="輸入 2 2" xfId="92" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="輸入 3 2" xfId="93" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="輸出 2 2" xfId="94" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="輸出 3 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="檢查儲存格 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="檢查儲存格 3 2" xfId="97" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="壞 2 2" xfId="98" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="壞 3 2" xfId="99" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="警告文字 2 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="警告文字 3 2" xfId="101" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1989,7 +1971,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="1RECORD"/>
@@ -2070,7 +2052,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="封面"/>
@@ -2177,9 +2159,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2217,9 +2199,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2254,7 +2236,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2289,7 +2271,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2462,7 +2444,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -2471,18 +2453,18 @@
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="4.90625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" style="8" customWidth="1"/>
     <col min="2" max="2" width="25" style="8" customWidth="1"/>
-    <col min="3" max="3" width="7.81640625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="10.6328125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="8" customWidth="1"/>
     <col min="5" max="6" width="22" style="8" customWidth="1"/>
-    <col min="7" max="7" width="36.81640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="36.77734375" style="8" customWidth="1"/>
     <col min="8" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="32.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2505,7 +2487,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="34">
+    <row r="2" spans="1:7" ht="32.4">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2526,7 +2508,7 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="51">
+    <row r="3" spans="1:7" ht="48.6">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2572,7 +2554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="51">
+    <row r="5" spans="1:7" ht="48.6">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2637,7 +2619,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="51">
+    <row r="8" spans="1:7" ht="48.6">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2726,7 +2708,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="34">
+    <row r="13" spans="1:7" ht="32.4">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2745,7 +2727,7 @@
       </c>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="34">
+    <row r="14" spans="1:7" ht="32.4">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2764,7 +2746,7 @@
       </c>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="34">
+    <row r="15" spans="1:7" ht="32.4">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2783,7 +2765,7 @@
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="34">
+    <row r="16" spans="1:7" ht="32.4">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2802,7 +2784,7 @@
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" ht="34">
+    <row r="17" spans="1:7" ht="32.4">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2821,7 +2803,7 @@
       </c>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" ht="34">
+    <row r="18" spans="1:7" ht="32.4">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2840,7 +2822,7 @@
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" ht="34">
+    <row r="19" spans="1:7" ht="32.4">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2865,13 +2847,13 @@
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="15"/>
-      <c r="F20" s="16"/>
-    </row>
-    <row r="21" spans="1:7" ht="34">
-      <c r="A21" s="17" t="s">
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" ht="32.4">
+      <c r="A21" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C21" s="14"/>
@@ -2880,72 +2862,69 @@
       <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="19"/>
-      <c r="B22" s="18" t="s">
+      <c r="A22" s="17"/>
+      <c r="B22" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A23" s="19"/>
-      <c r="B23" s="18" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="19" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="16"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="14"/>
       <c r="C25" s="14"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="16"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="14"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="14"/>
-      <c r="B26" s="18"/>
       <c r="C26" s="14"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="16"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="14"/>
-      <c r="B27" s="18"/>
       <c r="C27" s="14"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="16"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="16"/>
-      <c r="B28" s="18"/>
+      <c r="A28" s="14"/>
       <c r="C28" s="14"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="16"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:G24"/>
+  <autoFilter ref="B1:G24" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.56999999999999995" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="71" fitToHeight="2" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2959,7 +2938,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2969,541 +2948,490 @@
       <pane xSplit="5" ySplit="7" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="2.90625" style="38" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" style="38" customWidth="1"/>
-    <col min="3" max="3" width="9" style="38" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" style="38" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" style="38" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" style="38" customWidth="1"/>
-    <col min="7" max="7" width="26.1796875" style="38" customWidth="1"/>
-    <col min="8" max="8" width="24.90625" style="38" customWidth="1"/>
-    <col min="9" max="9" width="17.81640625" style="38" customWidth="1"/>
-    <col min="10" max="10" width="21.453125" style="38" customWidth="1"/>
-    <col min="11" max="12" width="12.6328125" style="38" customWidth="1"/>
-    <col min="13" max="13" width="17.90625" style="38" customWidth="1"/>
-    <col min="14" max="15" width="17.36328125" style="38" customWidth="1"/>
-    <col min="16" max="17" width="15.6328125" style="38" customWidth="1"/>
-    <col min="18" max="18" width="24.1796875" style="38" customWidth="1"/>
-    <col min="19" max="19" width="12.90625" style="38" customWidth="1"/>
-    <col min="20" max="16384" width="9" style="38"/>
+    <col min="1" max="1" width="2.88671875" style="34" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="34" customWidth="1"/>
+    <col min="3" max="3" width="9" style="34" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="34" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="34" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" style="34" customWidth="1"/>
+    <col min="7" max="7" width="26.21875" style="34" customWidth="1"/>
+    <col min="8" max="8" width="24.88671875" style="34" customWidth="1"/>
+    <col min="9" max="9" width="17.77734375" style="34" customWidth="1"/>
+    <col min="10" max="10" width="21.44140625" style="34" customWidth="1"/>
+    <col min="11" max="12" width="12.6640625" style="34" customWidth="1"/>
+    <col min="13" max="13" width="17.88671875" style="34" customWidth="1"/>
+    <col min="14" max="15" width="17.33203125" style="34" customWidth="1"/>
+    <col min="16" max="17" width="15.6640625" style="34" customWidth="1"/>
+    <col min="18" max="18" width="24.21875" style="34" customWidth="1"/>
+    <col min="19" max="19" width="12.88671875" style="34" customWidth="1"/>
+    <col min="20" max="16384" width="9" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24">
-      <c r="B1" s="38" t="s">
+    <row r="1" spans="2:19">
+      <c r="B1" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="34" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="2:24">
-      <c r="B2" s="38" t="s">
+    <row r="2" spans="2:19">
+      <c r="B2" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="69">
+      <c r="C2" s="64">
         <v>201909</v>
       </c>
     </row>
-    <row r="3" spans="2:24">
-      <c r="B3" s="38" t="s">
+    <row r="3" spans="2:19">
+      <c r="B3" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="R3" s="40"/>
-      <c r="S3" s="40" t="s">
+      <c r="R3" s="36"/>
+      <c r="S3" s="36" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="2:24">
-      <c r="B4" s="38" t="s">
+    <row r="4" spans="2:19">
+      <c r="B4" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="R4" s="36"/>
-      <c r="S4" s="37" t="s">
+      <c r="R4" s="32"/>
+      <c r="S4" s="33" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="2:24">
-      <c r="C5" s="39"/>
-      <c r="R5" s="36"/>
-      <c r="S5" s="37"/>
-    </row>
-    <row r="6" spans="2:24">
-      <c r="C6" s="39"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="71"/>
-    </row>
-    <row r="7" spans="2:24" s="42" customFormat="1" ht="51">
-      <c r="B7" s="41" t="s">
+    <row r="5" spans="2:19">
+      <c r="C5" s="35"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="33"/>
+    </row>
+    <row r="6" spans="2:19">
+      <c r="C6" s="35"/>
+      <c r="R6" s="66"/>
+      <c r="S6" s="66"/>
+    </row>
+    <row r="7" spans="2:19" s="38" customFormat="1" ht="48.6">
+      <c r="B7" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="41" t="s">
+      <c r="F7" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G7" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="41" t="s">
+      <c r="I7" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="J7" s="41" t="s">
+      <c r="J7" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="K7" s="41" t="s">
+      <c r="K7" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="L7" s="41" t="s">
+      <c r="L7" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="M7" s="41" t="s">
+      <c r="M7" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="N7" s="41" t="s">
+      <c r="N7" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="O7" s="41" t="s">
+      <c r="O7" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="P7" s="41" t="s">
+      <c r="P7" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="Q7" s="41" t="s">
+      <c r="Q7" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="R7" s="41" t="s">
+      <c r="R7" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="S7" s="41" t="s">
+      <c r="S7" s="37" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="2:24" s="46" customFormat="1" ht="15.5">
-      <c r="B8" s="43" t="s">
+    <row r="8" spans="2:19" s="42" customFormat="1" ht="15">
+      <c r="B8" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="63"/>
-      <c r="L8" s="63"/>
-      <c r="M8" s="63"/>
-      <c r="N8" s="63"/>
-      <c r="O8" s="63"/>
-      <c r="P8" s="63"/>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="64"/>
-      <c r="S8" s="45"/>
-    </row>
-    <row r="9" spans="2:24" s="46" customFormat="1" ht="15.5">
-      <c r="B9" s="43" t="s">
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="58"/>
+      <c r="Q8" s="58"/>
+      <c r="R8" s="59"/>
+      <c r="S8" s="41"/>
+    </row>
+    <row r="9" spans="2:19" s="42" customFormat="1" ht="15">
+      <c r="B9" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="63"/>
-      <c r="N9" s="63"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="63"/>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="64"/>
-      <c r="S9" s="45"/>
-    </row>
-    <row r="10" spans="2:24" s="49" customFormat="1" ht="15.5">
-      <c r="B10" s="43" t="s">
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="59"/>
+      <c r="S9" s="41"/>
+    </row>
+    <row r="10" spans="2:19" s="45" customFormat="1" ht="15">
+      <c r="B10" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="63"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="47"/>
-      <c r="P10" s="47"/>
-      <c r="Q10" s="65"/>
-      <c r="R10" s="66"/>
-      <c r="S10" s="48"/>
-    </row>
-    <row r="11" spans="2:24" s="49" customFormat="1" ht="15.5">
-      <c r="B11" s="43" t="s">
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="60"/>
+      <c r="R10" s="61"/>
+      <c r="S10" s="44"/>
+    </row>
+    <row r="11" spans="2:19" s="45" customFormat="1" ht="15">
+      <c r="B11" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="44" t="s">
+      <c r="E11" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="47"/>
-      <c r="P11" s="47"/>
-      <c r="Q11" s="65"/>
-      <c r="R11" s="67"/>
-      <c r="S11" s="50"/>
-    </row>
-    <row r="12" spans="2:24" s="49" customFormat="1">
-      <c r="B12" s="43" t="s">
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="60"/>
+      <c r="R11" s="62"/>
+      <c r="S11" s="46"/>
+    </row>
+    <row r="12" spans="2:19" s="45" customFormat="1">
+      <c r="B12" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="60"/>
+      <c r="R12" s="62"/>
+      <c r="S12" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="43" t="s">
+    </row>
+    <row r="13" spans="2:19" s="45" customFormat="1">
+      <c r="B13" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="63"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="47"/>
-      <c r="Q12" s="65"/>
-      <c r="R12" s="67"/>
-      <c r="S12" s="68" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="2:24" s="49" customFormat="1">
-      <c r="B13" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="44" t="s">
+      <c r="E13" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="63"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="47"/>
-      <c r="P13" s="47"/>
-      <c r="Q13" s="65"/>
-      <c r="R13" s="67"/>
-      <c r="S13" s="68"/>
-    </row>
-    <row r="14" spans="2:24" s="49" customFormat="1" ht="15.5">
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="52"/>
-      <c r="P14" s="52"/>
-      <c r="Q14" s="52"/>
-      <c r="R14" s="52"/>
-      <c r="S14" s="52"/>
-    </row>
-    <row r="15" spans="2:24" s="60" customFormat="1">
-      <c r="F15" s="62">
-        <f>SUM(F8:F14)</f>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="60"/>
+      <c r="R13" s="62"/>
+      <c r="S13" s="63"/>
+    </row>
+    <row r="14" spans="2:19" s="45" customFormat="1" ht="15">
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="48"/>
+      <c r="S14" s="48"/>
+    </row>
+    <row r="15" spans="2:19" s="55" customFormat="1">
+      <c r="F15" s="57">
+        <f t="shared" ref="F15:Q15" si="0">SUM(F8:F14)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="62">
-        <f>SUM(G8:G14)</f>
+      <c r="G15" s="57">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H15" s="62">
-        <f>SUM(H8:H14)</f>
+      <c r="H15" s="57">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="62">
-        <f>SUM(I8:I14)</f>
+      <c r="I15" s="57">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J15" s="62">
-        <f>SUM(J8:J14)</f>
+      <c r="J15" s="57">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K15" s="62">
-        <f>SUM(K8:K14)</f>
+      <c r="K15" s="57">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L15" s="62">
-        <f>SUM(L8:L14)</f>
+      <c r="L15" s="57">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M15" s="62">
-        <f>SUM(M8:M14)</f>
+      <c r="M15" s="57">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N15" s="62">
-        <f>SUM(N8:N14)</f>
+      <c r="N15" s="57">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O15" s="62">
-        <f>SUM(O8:O14)</f>
+      <c r="O15" s="57">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P15" s="62">
-        <f>SUM(P8:P14)</f>
+      <c r="P15" s="57">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q15" s="62">
-        <f>SUM(Q8:Q14)</f>
+      <c r="Q15" s="57">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R15" s="61"/>
-    </row>
-    <row r="16" spans="2:24">
-      <c r="B16" s="53" t="s">
+      <c r="R15" s="56"/>
+    </row>
+    <row r="16" spans="2:19">
+      <c r="B16" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="56"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="56"/>
-      <c r="R16" s="53"/>
-      <c r="S16" s="53"/>
-      <c r="T16" s="53"/>
-      <c r="U16" s="53"/>
-      <c r="V16" s="53"/>
-      <c r="W16" s="53"/>
-      <c r="X16" s="53"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="49"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="51"/>
     </row>
     <row r="17" spans="1:25">
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="53"/>
-      <c r="P17" s="53"/>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="53"/>
-      <c r="S17" s="53"/>
-      <c r="T17" s="53"/>
-      <c r="U17" s="53"/>
-      <c r="V17" s="53"/>
-      <c r="W17" s="53"/>
-      <c r="X17" s="53"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="53"/>
     </row>
     <row r="18" spans="1:25" ht="35.25" customHeight="1">
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="65" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="70"/>
-      <c r="M18" s="70"/>
-      <c r="N18" s="70"/>
-      <c r="O18" s="70"/>
-      <c r="P18" s="70"/>
-      <c r="Q18" s="70"/>
-      <c r="R18" s="70"/>
-      <c r="S18" s="70"/>
-      <c r="T18" s="58"/>
-      <c r="U18" s="58"/>
-      <c r="V18" s="58"/>
-      <c r="W18" s="58"/>
-      <c r="X18" s="58"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="65"/>
+      <c r="N18" s="65"/>
+      <c r="O18" s="65"/>
+      <c r="P18" s="65"/>
+      <c r="Q18" s="65"/>
+      <c r="R18" s="65"/>
+      <c r="S18" s="65"/>
+      <c r="T18" s="53"/>
+      <c r="U18" s="53"/>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="53"/>
     </row>
     <row r="19" spans="1:25" ht="16.5" customHeight="1">
-      <c r="B19" s="70" t="s">
+      <c r="B19" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="70"/>
-      <c r="J19" s="70"/>
-      <c r="K19" s="70"/>
-      <c r="L19" s="70"/>
-      <c r="M19" s="70"/>
-      <c r="N19" s="70"/>
-      <c r="O19" s="70"/>
-      <c r="P19" s="70"/>
-      <c r="Q19" s="70"/>
-      <c r="R19" s="70"/>
-      <c r="S19" s="58"/>
-      <c r="T19" s="58"/>
-      <c r="U19" s="58"/>
-      <c r="V19" s="58"/>
-      <c r="W19" s="58"/>
-      <c r="X19" s="58"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="65"/>
+      <c r="M19" s="65"/>
+      <c r="N19" s="65"/>
+      <c r="O19" s="65"/>
+      <c r="P19" s="65"/>
+      <c r="Q19" s="65"/>
+      <c r="R19" s="65"/>
+      <c r="S19" s="53"/>
+      <c r="T19" s="53"/>
+      <c r="U19" s="53"/>
+      <c r="V19" s="53"/>
+      <c r="W19" s="53"/>
+      <c r="X19" s="53"/>
     </row>
     <row r="20" spans="1:25">
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="53"/>
-      <c r="N20" s="53"/>
-      <c r="O20" s="53"/>
-      <c r="P20" s="53"/>
-      <c r="Q20" s="53"/>
-      <c r="R20" s="53"/>
-      <c r="S20" s="53"/>
-      <c r="T20" s="53"/>
-      <c r="U20" s="53"/>
-      <c r="V20" s="53"/>
-      <c r="W20" s="53"/>
-      <c r="X20" s="53"/>
     </row>
     <row r="21" spans="1:25">
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="34" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:25" s="26" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A23" s="59"/>
-      <c r="B23" s="26" t="s">
+    <row r="23" spans="1:25" s="23" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A23" s="54"/>
+      <c r="B23" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="28"/>
-      <c r="G23" s="31"/>
-      <c r="I23" s="31" t="s">
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="G23" s="27"/>
+      <c r="I23" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="J23" s="29"/>
-      <c r="K23" s="30"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="26" t="s">
+      <c r="J23" s="25"/>
+      <c r="K23" s="26"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="Q23" s="32"/>
-      <c r="R23" s="33"/>
-      <c r="T23" s="34"/>
-      <c r="W23" s="35"/>
-      <c r="Y23" s="26" t="s">
+      <c r="Q23" s="28"/>
+      <c r="R23" s="29"/>
+      <c r="T23" s="30"/>
+      <c r="W23" s="31"/>
+      <c r="Y23" s="23" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto-committed on 2023/09/25 週一 14:57:22.16
</commit_message>
<xml_diff>
--- a/Program/Other/LM055_底稿_A042放款餘額彙總表.xlsx
+++ b/Program/Other/LM055_底稿_A042放款餘額彙總表.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SKL_SVN\iTX\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA8428B-558B-4136-8532-8D3CA8E1608C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A042填報說明" sheetId="1" r:id="rId1"/>
@@ -75,7 +74,7 @@
     <definedName name="TextRefCopyRangeCount" hidden="1">46</definedName>
     <definedName name="新">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -737,8 +736,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="9">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
@@ -747,6 +746,7 @@
     <numFmt numFmtId="179" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="180" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="181" formatCode="#,##0.0000_);[Red]\(#,##0.0000\)"/>
+    <numFmt numFmtId="182" formatCode="#,##0_);[Red]\(#,##0\)"/>
   </numFmts>
   <fonts count="37">
     <font>
@@ -1651,7 +1651,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1825,137 +1825,134 @@
     <xf numFmtId="177" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="3" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="3" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="2" xfId="49" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="2" xfId="49" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="2" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="8" fillId="0" borderId="2" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="182" fontId="15" fillId="0" borderId="3" xfId="49" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="15" fillId="0" borderId="2" xfId="49" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="15" fillId="0" borderId="2" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="182" fontId="15" fillId="0" borderId="3" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="102">
-    <cellStyle name="20% - 輔色1 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - 輔色1 3 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - 輔色2 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - 輔色2 3 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - 輔色3 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - 輔色3 3 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="20% - 輔色4 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="20% - 輔色4 3 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="20% - 輔色5 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="20% - 輔色5 3 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="20% - 輔色6 2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="20% - 輔色6 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="40% - 輔色1 2 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="40% - 輔色1 3 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="40% - 輔色2 2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="40% - 輔色2 3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="40% - 輔色3 2 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="40% - 輔色3 3 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="40% - 輔色4 2 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="40% - 輔色4 3 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="40% - 輔色5 2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="40% - 輔色5 3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="40% - 輔色6 2 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="40% - 輔色6 3 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="60% - 輔色1 2 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="60% - 輔色1 3 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="60% - 輔色2 2 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="60% - 輔色2 3 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="60% - 輔色3 2 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="60% - 輔色3 3 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="60% - 輔色4 2 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="60% - 輔色4 3 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="60% - 輔色5 2 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="60% - 輔色5 3 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="60% - 輔色6 2 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="60% - 輔色6 3 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="20% - 輔色1 2 2" xfId="1"/>
+    <cellStyle name="20% - 輔色1 3 2" xfId="2"/>
+    <cellStyle name="20% - 輔色2 2 2" xfId="3"/>
+    <cellStyle name="20% - 輔色2 3 2" xfId="4"/>
+    <cellStyle name="20% - 輔色3 2 2" xfId="5"/>
+    <cellStyle name="20% - 輔色3 3 2" xfId="6"/>
+    <cellStyle name="20% - 輔色4 2 2" xfId="7"/>
+    <cellStyle name="20% - 輔色4 3 2" xfId="8"/>
+    <cellStyle name="20% - 輔色5 2 2" xfId="9"/>
+    <cellStyle name="20% - 輔色5 3 2" xfId="10"/>
+    <cellStyle name="20% - 輔色6 2 2" xfId="11"/>
+    <cellStyle name="20% - 輔色6 3 2" xfId="12"/>
+    <cellStyle name="40% - 輔色1 2 2" xfId="13"/>
+    <cellStyle name="40% - 輔色1 3 2" xfId="14"/>
+    <cellStyle name="40% - 輔色2 2 2" xfId="15"/>
+    <cellStyle name="40% - 輔色2 3 2" xfId="16"/>
+    <cellStyle name="40% - 輔色3 2 2" xfId="17"/>
+    <cellStyle name="40% - 輔色3 3 2" xfId="18"/>
+    <cellStyle name="40% - 輔色4 2 2" xfId="19"/>
+    <cellStyle name="40% - 輔色4 3 2" xfId="20"/>
+    <cellStyle name="40% - 輔色5 2 2" xfId="21"/>
+    <cellStyle name="40% - 輔色5 3 2" xfId="22"/>
+    <cellStyle name="40% - 輔色6 2 2" xfId="23"/>
+    <cellStyle name="40% - 輔色6 3 2" xfId="24"/>
+    <cellStyle name="60% - 輔色1 2 2" xfId="25"/>
+    <cellStyle name="60% - 輔色1 3 2" xfId="26"/>
+    <cellStyle name="60% - 輔色2 2 2" xfId="27"/>
+    <cellStyle name="60% - 輔色2 3 2" xfId="28"/>
+    <cellStyle name="60% - 輔色3 2 2" xfId="29"/>
+    <cellStyle name="60% - 輔色3 3 2" xfId="30"/>
+    <cellStyle name="60% - 輔色4 2 2" xfId="31"/>
+    <cellStyle name="60% - 輔色4 3 2" xfId="32"/>
+    <cellStyle name="60% - 輔色5 2 2" xfId="33"/>
+    <cellStyle name="60% - 輔色5 3 2" xfId="34"/>
+    <cellStyle name="60% - 輔色6 2 2" xfId="35"/>
+    <cellStyle name="60% - 輔色6 3 2" xfId="36"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 10" xfId="37" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="一般 10 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="一般 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="一般 2 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="一般 3" xfId="41" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="一般 3 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="一般 4" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="一般 5" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="一般 6" xfId="45" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="一般_921002保險業月報yaotung" xfId="46" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="一般_9211預月" xfId="47" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="一般_半年報檢查報表-壽險" xfId="48" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="一般 10" xfId="37"/>
+    <cellStyle name="一般 10 2" xfId="38"/>
+    <cellStyle name="一般 2" xfId="39"/>
+    <cellStyle name="一般 2 2" xfId="40"/>
+    <cellStyle name="一般 3" xfId="41"/>
+    <cellStyle name="一般 3 2" xfId="42"/>
+    <cellStyle name="一般 4" xfId="43"/>
+    <cellStyle name="一般 5" xfId="44"/>
+    <cellStyle name="一般 6" xfId="45"/>
+    <cellStyle name="一般_921002保險業月報yaotung" xfId="46"/>
+    <cellStyle name="一般_9211預月" xfId="47"/>
+    <cellStyle name="一般_半年報檢查報表-壽險" xfId="48"/>
     <cellStyle name="千分位" xfId="49" builtinId="3"/>
-    <cellStyle name="千分位 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="千分位 3" xfId="51" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="千分位 3 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="千分位 4" xfId="53" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="千分位[0] 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="中等 2 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="中等 3 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="合計 2 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="合計 3 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="好 2 2" xfId="59" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="好 3 2" xfId="60" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="百分比 2" xfId="61" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="計算方式 2 2" xfId="62" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="計算方式 3 2" xfId="63" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="連結的儲存格 2 2" xfId="64" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="連結的儲存格 3 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="備註 2 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="備註 3 2" xfId="67" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="說明文字 2 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="說明文字 3 2" xfId="69" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="輔色1 2 2" xfId="70" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="輔色1 3 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="輔色2 2 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="輔色2 3 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="輔色3 2 2" xfId="74" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="輔色3 3 2" xfId="75" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="輔色4 2 2" xfId="76" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="輔色4 3 2" xfId="77" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="輔色5 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="輔色5 3 2" xfId="79" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="輔色6 2 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="輔色6 3 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="標題 1 2 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="標題 1 3 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="標題 2 2 2" xfId="84" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="標題 2 3 2" xfId="85" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="標題 3 2 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="標題 3 3 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="標題 4 2 2" xfId="88" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="標題 4 3 2" xfId="89" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="標題 5 2" xfId="90" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="標題 6 2" xfId="91" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="輸入 2 2" xfId="92" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="輸入 3 2" xfId="93" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="輸出 2 2" xfId="94" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="輸出 3 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="檢查儲存格 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="檢查儲存格 3 2" xfId="97" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="壞 2 2" xfId="98" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="壞 3 2" xfId="99" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="警告文字 2 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="警告文字 3 2" xfId="101" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="千分位 2" xfId="50"/>
+    <cellStyle name="千分位 3" xfId="51"/>
+    <cellStyle name="千分位 3 2" xfId="52"/>
+    <cellStyle name="千分位 4" xfId="53"/>
+    <cellStyle name="千分位[0] 2" xfId="54"/>
+    <cellStyle name="中等 2 2" xfId="55"/>
+    <cellStyle name="中等 3 2" xfId="56"/>
+    <cellStyle name="合計 2 2" xfId="57"/>
+    <cellStyle name="合計 3 2" xfId="58"/>
+    <cellStyle name="好 2 2" xfId="59"/>
+    <cellStyle name="好 3 2" xfId="60"/>
+    <cellStyle name="百分比 2" xfId="61"/>
+    <cellStyle name="計算方式 2 2" xfId="62"/>
+    <cellStyle name="計算方式 3 2" xfId="63"/>
+    <cellStyle name="連結的儲存格 2 2" xfId="64"/>
+    <cellStyle name="連結的儲存格 3 2" xfId="65"/>
+    <cellStyle name="備註 2 2" xfId="66"/>
+    <cellStyle name="備註 3 2" xfId="67"/>
+    <cellStyle name="說明文字 2 2" xfId="68"/>
+    <cellStyle name="說明文字 3 2" xfId="69"/>
+    <cellStyle name="輔色1 2 2" xfId="70"/>
+    <cellStyle name="輔色1 3 2" xfId="71"/>
+    <cellStyle name="輔色2 2 2" xfId="72"/>
+    <cellStyle name="輔色2 3 2" xfId="73"/>
+    <cellStyle name="輔色3 2 2" xfId="74"/>
+    <cellStyle name="輔色3 3 2" xfId="75"/>
+    <cellStyle name="輔色4 2 2" xfId="76"/>
+    <cellStyle name="輔色4 3 2" xfId="77"/>
+    <cellStyle name="輔色5 2 2" xfId="78"/>
+    <cellStyle name="輔色5 3 2" xfId="79"/>
+    <cellStyle name="輔色6 2 2" xfId="80"/>
+    <cellStyle name="輔色6 3 2" xfId="81"/>
+    <cellStyle name="標題 1 2 2" xfId="82"/>
+    <cellStyle name="標題 1 3 2" xfId="83"/>
+    <cellStyle name="標題 2 2 2" xfId="84"/>
+    <cellStyle name="標題 2 3 2" xfId="85"/>
+    <cellStyle name="標題 3 2 2" xfId="86"/>
+    <cellStyle name="標題 3 3 2" xfId="87"/>
+    <cellStyle name="標題 4 2 2" xfId="88"/>
+    <cellStyle name="標題 4 3 2" xfId="89"/>
+    <cellStyle name="標題 5 2" xfId="90"/>
+    <cellStyle name="標題 6 2" xfId="91"/>
+    <cellStyle name="輸入 2 2" xfId="92"/>
+    <cellStyle name="輸入 3 2" xfId="93"/>
+    <cellStyle name="輸出 2 2" xfId="94"/>
+    <cellStyle name="輸出 3 2" xfId="95"/>
+    <cellStyle name="檢查儲存格 2 2" xfId="96"/>
+    <cellStyle name="檢查儲存格 3 2" xfId="97"/>
+    <cellStyle name="壞 2 2" xfId="98"/>
+    <cellStyle name="壞 3 2" xfId="99"/>
+    <cellStyle name="警告文字 2 2" xfId="100"/>
+    <cellStyle name="警告文字 3 2" xfId="101"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1971,7 +1968,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="1RECORD"/>
@@ -2052,7 +2049,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="封面"/>
@@ -2105,11 +2102,41 @@
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
+      <sheetData sheetId="3">
+        <row r="6">
+          <cell r="E6">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="8">
+          <cell r="C8">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
+        <row r="6">
+          <cell r="C6">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6">
+        <row r="21">
+          <cell r="C21">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7">
+        <row r="28">
+          <cell r="C28">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
@@ -2117,9 +2144,20 @@
       <sheetData sheetId="12"/>
       <sheetData sheetId="13"/>
       <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
+      <sheetData sheetId="15">
+        <row r="25">
+          <cell r="O25">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="16"/>
       <sheetData sheetId="17">
+        <row r="8">
+          <cell r="G8">
+            <v>0</v>
+          </cell>
+        </row>
         <row r="44">
           <cell r="G44">
             <v>0</v>
@@ -2141,7 +2179,13 @@
       <sheetData sheetId="30"/>
       <sheetData sheetId="31"/>
       <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
+      <sheetData sheetId="33">
+        <row r="7">
+          <cell r="E7">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="34"/>
       <sheetData sheetId="35"/>
       <sheetData sheetId="36"/>
@@ -2159,9 +2203,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2199,9 +2243,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2236,7 +2280,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2271,7 +2315,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2444,7 +2488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -2924,7 +2968,7 @@
       <c r="F28" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:G24" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:G24"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.56999999999999995" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="71" fitToHeight="2" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -2938,7 +2982,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2948,7 +2992,7 @@
       <pane xSplit="5" ySplit="7" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
@@ -2960,8 +3004,8 @@
     <col min="5" max="5" width="21.33203125" style="34" customWidth="1"/>
     <col min="6" max="6" width="17.77734375" style="34" customWidth="1"/>
     <col min="7" max="7" width="26.21875" style="34" customWidth="1"/>
-    <col min="8" max="8" width="24.88671875" style="34" customWidth="1"/>
-    <col min="9" max="9" width="17.77734375" style="34" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" style="34" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" style="34" customWidth="1"/>
     <col min="10" max="10" width="21.44140625" style="34" customWidth="1"/>
     <col min="11" max="12" width="12.6640625" style="34" customWidth="1"/>
     <col min="13" max="13" width="17.88671875" style="34" customWidth="1"/>
@@ -2984,7 +3028,7 @@
       <c r="B2" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="64">
+      <c r="C2" s="59">
         <v>201909</v>
       </c>
     </row>
@@ -3019,8 +3063,8 @@
     </row>
     <row r="6" spans="2:19">
       <c r="C6" s="35"/>
-      <c r="R6" s="66"/>
-      <c r="S6" s="66"/>
+      <c r="R6" s="64"/>
+      <c r="S6" s="64"/>
     </row>
     <row r="7" spans="2:19" s="38" customFormat="1" ht="48.6">
       <c r="B7" s="37" t="s">
@@ -3091,19 +3135,19 @@
       <c r="E8" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="58"/>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="58"/>
-      <c r="R8" s="59"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
+      <c r="N8" s="65"/>
+      <c r="O8" s="65"/>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="65"/>
+      <c r="R8" s="65"/>
       <c r="S8" s="41"/>
     </row>
     <row r="9" spans="2:19" s="42" customFormat="1" ht="15">
@@ -3119,19 +3163,19 @@
       <c r="E9" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="58"/>
-      <c r="Q9" s="58"/>
-      <c r="R9" s="59"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="65"/>
+      <c r="N9" s="65"/>
+      <c r="O9" s="65"/>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="65"/>
+      <c r="R9" s="65"/>
       <c r="S9" s="41"/>
     </row>
     <row r="10" spans="2:19" s="45" customFormat="1" ht="15">
@@ -3147,18 +3191,18 @@
       <c r="E10" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="43"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="43"/>
-      <c r="Q10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="60"/>
+      <c r="Q10" s="61"/>
       <c r="R10" s="61"/>
       <c r="S10" s="44"/>
     </row>
@@ -3175,18 +3219,18 @@
       <c r="E11" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="60"/>
+      <c r="Q11" s="61"/>
       <c r="R11" s="62"/>
       <c r="S11" s="46"/>
     </row>
@@ -3203,20 +3247,20 @@
       <c r="E12" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="43"/>
-      <c r="Q12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="60"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="61"/>
       <c r="R12" s="62"/>
-      <c r="S12" s="63" t="s">
+      <c r="S12" s="58" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3233,20 +3277,20 @@
       <c r="E13" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="60"/>
+      <c r="P13" s="60"/>
+      <c r="Q13" s="61"/>
       <c r="R13" s="62"/>
-      <c r="S13" s="63"/>
+      <c r="S13" s="58"/>
     </row>
     <row r="14" spans="2:19" s="45" customFormat="1" ht="15">
       <c r="B14" s="39"/>
@@ -3345,26 +3389,26 @@
       <c r="H17" s="53"/>
     </row>
     <row r="18" spans="1:25" ht="35.25" customHeight="1">
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="65"/>
-      <c r="N18" s="65"/>
-      <c r="O18" s="65"/>
-      <c r="P18" s="65"/>
-      <c r="Q18" s="65"/>
-      <c r="R18" s="65"/>
-      <c r="S18" s="65"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="63"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="63"/>
+      <c r="R18" s="63"/>
+      <c r="S18" s="63"/>
       <c r="T18" s="53"/>
       <c r="U18" s="53"/>
       <c r="V18" s="53"/>
@@ -3372,25 +3416,25 @@
       <c r="X18" s="53"/>
     </row>
     <row r="19" spans="1:25" ht="16.5" customHeight="1">
-      <c r="B19" s="65" t="s">
+      <c r="B19" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="65"/>
-      <c r="M19" s="65"/>
-      <c r="N19" s="65"/>
-      <c r="O19" s="65"/>
-      <c r="P19" s="65"/>
-      <c r="Q19" s="65"/>
-      <c r="R19" s="65"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="63"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="63"/>
+      <c r="R19" s="63"/>
       <c r="S19" s="53"/>
       <c r="T19" s="53"/>
       <c r="U19" s="53"/>

</xml_diff>

<commit_message>
Auto-committed on 2023/10/05 週四 16:43:13.01
</commit_message>
<xml_diff>
--- a/Program/Other/LM055_底稿_A042放款餘額彙總表.xlsx
+++ b/Program/Other/LM055_底稿_A042放款餘額彙總表.xlsx
@@ -5,7 +5,7 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\SKL\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1651,7 +1651,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1780,9 +1780,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="3" xfId="49" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="15" fillId="0" borderId="2" xfId="49" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1819,12 +1816,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="8" fillId="0" borderId="2" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1840,13 +1831,19 @@
     <xf numFmtId="182" fontId="15" fillId="0" borderId="2" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="182" fontId="15" fillId="0" borderId="3" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="15" fillId="0" borderId="3" xfId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="2" xfId="49" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="15" fillId="0" borderId="0" xfId="49" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2989,10 +2986,10 @@
   <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="7" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="7" topLeftCell="K8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2"/>
@@ -3028,7 +3025,7 @@
       <c r="B2" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="59">
+      <c r="C2" s="56">
         <v>201909</v>
       </c>
     </row>
@@ -3063,8 +3060,8 @@
     </row>
     <row r="6" spans="2:19">
       <c r="C6" s="35"/>
-      <c r="R6" s="64"/>
-      <c r="S6" s="64"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="62"/>
     </row>
     <row r="7" spans="2:19" s="38" customFormat="1" ht="48.6">
       <c r="B7" s="37" t="s">
@@ -3135,19 +3132,19 @@
       <c r="E8" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="65"/>
-      <c r="O8" s="65"/>
-      <c r="P8" s="65"/>
-      <c r="Q8" s="65"/>
-      <c r="R8" s="65"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
+      <c r="R8" s="60"/>
       <c r="S8" s="41"/>
     </row>
     <row r="9" spans="2:19" s="42" customFormat="1" ht="15">
@@ -3163,22 +3160,22 @@
       <c r="E9" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="65"/>
-      <c r="O9" s="65"/>
-      <c r="P9" s="65"/>
-      <c r="Q9" s="65"/>
-      <c r="R9" s="65"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="60"/>
+      <c r="R9" s="60"/>
       <c r="S9" s="41"/>
     </row>
-    <row r="10" spans="2:19" s="45" customFormat="1" ht="15">
+    <row r="10" spans="2:19" s="44" customFormat="1" ht="15">
       <c r="B10" s="39" t="s">
         <v>86</v>
       </c>
@@ -3191,22 +3188,22 @@
       <c r="E10" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="61"/>
-      <c r="R10" s="61"/>
-      <c r="S10" s="44"/>
-    </row>
-    <row r="11" spans="2:19" s="45" customFormat="1" ht="15">
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="57"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="43"/>
+    </row>
+    <row r="11" spans="2:19" s="44" customFormat="1" ht="15">
       <c r="B11" s="39" t="s">
         <v>87</v>
       </c>
@@ -3219,22 +3216,22 @@
       <c r="E11" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="60"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="61"/>
-      <c r="R11" s="62"/>
-      <c r="S11" s="46"/>
-    </row>
-    <row r="12" spans="2:19" s="45" customFormat="1">
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="59"/>
+      <c r="S11" s="45"/>
+    </row>
+    <row r="12" spans="2:19" s="44" customFormat="1">
       <c r="B12" s="39" t="s">
         <v>86</v>
       </c>
@@ -3244,27 +3241,27 @@
       <c r="D12" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="47" t="s">
+      <c r="E12" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="60"/>
-      <c r="O12" s="60"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="61"/>
-      <c r="R12" s="62"/>
-      <c r="S12" s="58" t="s">
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="57"/>
+      <c r="P12" s="57"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="59"/>
+      <c r="S12" s="55" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="2:19" s="45" customFormat="1">
+    <row r="13" spans="2:19" s="44" customFormat="1">
       <c r="B13" s="39" t="s">
         <v>86</v>
       </c>
@@ -3277,170 +3274,173 @@
       <c r="E13" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="61"/>
-      <c r="R13" s="62"/>
-      <c r="S13" s="58"/>
-    </row>
-    <row r="14" spans="2:19" s="45" customFormat="1" ht="15">
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="57"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="59"/>
+      <c r="S13" s="55"/>
+    </row>
+    <row r="14" spans="2:19" s="44" customFormat="1" ht="15">
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
       <c r="E14" s="40"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="48"/>
-      <c r="S14" s="48"/>
-    </row>
-    <row r="15" spans="2:19" s="55" customFormat="1">
-      <c r="F15" s="57">
-        <f t="shared" ref="F15:Q15" si="0">SUM(F8:F14)</f>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="47"/>
+      <c r="R14" s="47"/>
+      <c r="S14" s="47"/>
+    </row>
+    <row r="15" spans="2:19" s="54" customFormat="1">
+      <c r="F15" s="64">
+        <f t="shared" ref="F15:R15" si="0">SUM(F8:F14)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="57">
+      <c r="G15" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H15" s="57">
+      <c r="H15" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="57">
+      <c r="I15" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J15" s="57">
+      <c r="J15" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K15" s="57">
+      <c r="K15" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L15" s="57">
+      <c r="L15" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M15" s="57">
+      <c r="M15" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N15" s="57">
+      <c r="N15" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O15" s="57">
+      <c r="O15" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P15" s="57">
+      <c r="P15" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q15" s="57">
+      <c r="Q15" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R15" s="56"/>
+      <c r="R15" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="49"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="51"/>
-      <c r="P16" s="51"/>
-      <c r="Q16" s="51"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="48"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="50"/>
+      <c r="P16" s="50"/>
+      <c r="Q16" s="50"/>
     </row>
     <row r="17" spans="1:25">
       <c r="B17" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="53"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="52"/>
     </row>
     <row r="18" spans="1:25" ht="35.25" customHeight="1">
-      <c r="B18" s="63" t="s">
+      <c r="B18" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="63"/>
-      <c r="K18" s="63"/>
-      <c r="L18" s="63"/>
-      <c r="M18" s="63"/>
-      <c r="N18" s="63"/>
-      <c r="O18" s="63"/>
-      <c r="P18" s="63"/>
-      <c r="Q18" s="63"/>
-      <c r="R18" s="63"/>
-      <c r="S18" s="63"/>
-      <c r="T18" s="53"/>
-      <c r="U18" s="53"/>
-      <c r="V18" s="53"/>
-      <c r="W18" s="53"/>
-      <c r="X18" s="53"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="61"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="61"/>
+      <c r="P18" s="61"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="52"/>
+      <c r="U18" s="52"/>
+      <c r="V18" s="52"/>
+      <c r="W18" s="52"/>
+      <c r="X18" s="52"/>
     </row>
     <row r="19" spans="1:25" ht="16.5" customHeight="1">
-      <c r="B19" s="63" t="s">
+      <c r="B19" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="63"/>
-      <c r="K19" s="63"/>
-      <c r="L19" s="63"/>
-      <c r="M19" s="63"/>
-      <c r="N19" s="63"/>
-      <c r="O19" s="63"/>
-      <c r="P19" s="63"/>
-      <c r="Q19" s="63"/>
-      <c r="R19" s="63"/>
-      <c r="S19" s="53"/>
-      <c r="T19" s="53"/>
-      <c r="U19" s="53"/>
-      <c r="V19" s="53"/>
-      <c r="W19" s="53"/>
-      <c r="X19" s="53"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="61"/>
+      <c r="L19" s="61"/>
+      <c r="M19" s="61"/>
+      <c r="N19" s="61"/>
+      <c r="O19" s="61"/>
+      <c r="P19" s="61"/>
+      <c r="Q19" s="61"/>
+      <c r="R19" s="61"/>
+      <c r="S19" s="52"/>
+      <c r="T19" s="52"/>
+      <c r="U19" s="52"/>
+      <c r="V19" s="52"/>
+      <c r="W19" s="52"/>
+      <c r="X19" s="52"/>
     </row>
     <row r="20" spans="1:25">
       <c r="B20" s="34" t="s">
@@ -3453,7 +3453,7 @@
       </c>
     </row>
     <row r="23" spans="1:25" s="23" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A23" s="54"/>
+      <c r="A23" s="53"/>
       <c r="B23" s="23" t="s">
         <v>93</v>
       </c>

</xml_diff>